<commit_message>
resnet34 / resnet50 training on cropped images
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t xml:space="preserve">https://www.crowdanalytix.com/contests/gamma-log-facies-type-prediction</t>
   </si>
@@ -171,6 +171,24 @@
   </si>
   <si>
     <t xml:space="preserve">1 cycle only then nan, ran script 02_07_3_unet_masked_6_colour_crop_facies.py  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Images re-generated at 2200x512 pixels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training on 1100 x 256, with 256x256 crops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_10_3_256_resnet50_masked_tab20_crop_val_set_0.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resnet50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02_10_4_256_resnet34_masked_tab20_crop_dice_val_set_1.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Needs work on combo loss function</t>
   </si>
 </sst>
 </file>
@@ -181,11 +199,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -204,94 +223,19 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,48 +244,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <fgColor rgb="FFF7A19A"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -349,23 +257,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -389,68 +282,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -462,46 +304,33 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -513,7 +342,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -527,9 +356,9 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFF7A19A"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -588,10 +417,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AMJ12"/>
+  <dimension ref="A1:AMJ21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -894,6 +723,32 @@
         <v>49</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>